<commit_message>
chapter 46, course 1
</commit_message>
<xml_diff>
--- a/Performance advises.xlsx
+++ b/Performance advises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sewer\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5B6BF4-790E-4642-85FC-80D7F3B55824}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B635C76F-AEF0-40A3-A3A0-88344AE58142}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10704" xr2:uid="{9726E777-4741-4EE5-B2A9-524597499CAB}"/>
   </bookViews>
@@ -25,21 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
-  <si>
-    <t>Prefer</t>
-  </si>
-  <si>
-    <t>Not to do</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="70">
   <si>
     <t xml:space="preserve">prefer GROUP BY </t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>not window functions</t>
   </si>
   <si>
     <t>prefer SELECT field</t>
@@ -198,14 +189,65 @@
     <t>BETWEEN</t>
   </si>
   <si>
-    <t>&lt;= &gt;=</t>
+    <t>SLOW</t>
+  </si>
+  <si>
+    <t>window functions</t>
+  </si>
+  <si>
+    <t>FAST ALTERNATIVE</t>
+  </si>
+  <si>
+    <t>CTE</t>
+  </si>
+  <si>
+    <t>Temp table</t>
+  </si>
+  <si>
+    <t>Appropriate Naming Convention</t>
+  </si>
+  <si>
+    <t>UNION ALL</t>
+  </si>
+  <si>
+    <t>UNION</t>
+  </si>
+  <si>
+    <t>Count(*) and Count(Column_Name)</t>
+  </si>
+  <si>
+    <t>Use Count(1)</t>
+  </si>
+  <si>
+    <t>&lt;= &gt;=  IN</t>
+  </si>
+  <si>
+    <t>Cursor</t>
+  </si>
+  <si>
+    <t>Select logic</t>
+  </si>
+  <si>
+    <t>Drop Index before Bulk Insertion of Data</t>
+  </si>
+  <si>
+    <t>Use Unique Constraint and Check Constraint</t>
+  </si>
+  <si>
+    <t>Avoid Loops In Coding</t>
+  </si>
+  <si>
+    <t>Avoid Correlated Queries</t>
+  </si>
+  <si>
+    <t>Use Index for required columns (SARG)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,18 +259,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF323232"/>
-      <name val="Calibri"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="4">
@@ -263,21 +329,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A286D64-563E-4094-9655-AF5C5DE73EA8}">
-  <dimension ref="B2:D45"/>
+  <dimension ref="B2:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,292 +696,360 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="3"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
-      <c r="C33" s="4" t="s">
-        <v>45</v>
+      <c r="C33" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="6"/>
-      <c r="C39" s="4"/>
+      <c r="C39" s="3"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="6"/>
-      <c r="C40" s="4"/>
+      <c r="C40" s="3"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" s="6"/>
-      <c r="C41" s="4"/>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" s="6"/>
-      <c r="C42" s="4"/>
+      <c r="C42" s="3"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" s="6"/>
-      <c r="C43" s="4"/>
+      <c r="C43" s="3"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" s="6"/>
-      <c r="C44" s="4"/>
+      <c r="C44" s="3"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="7" t="s">
         <v>55</v>
       </c>
+      <c r="C46" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B47" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B51" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B52" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B53" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B54" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B55" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
course 2 + videos yt
</commit_message>
<xml_diff>
--- a/Performance advises.xlsx
+++ b/Performance advises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sewer\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B635C76F-AEF0-40A3-A3A0-88344AE58142}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A495877-98BE-4D4C-897E-0D3A3F4A0462}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10704" xr2:uid="{9726E777-4741-4EE5-B2A9-524597499CAB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t xml:space="preserve">prefer GROUP BY </t>
   </si>
@@ -241,6 +241,18 @@
   </si>
   <si>
     <t>Use Index for required columns (SARG)</t>
+  </si>
+  <si>
+    <t>partition view with UNIONs</t>
+  </si>
+  <si>
+    <t>view with UNIONs</t>
+  </si>
+  <si>
+    <t>nested views</t>
+  </si>
+  <si>
+    <t>stored procedures</t>
   </si>
 </sst>
 </file>
@@ -338,9 +350,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -348,6 +357,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A286D64-563E-4094-9655-AF5C5DE73EA8}">
-  <dimension ref="B2:D55"/>
+  <dimension ref="B2:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,37 +958,37 @@
       </c>
     </row>
     <row r="38" spans="2:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="6"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="6"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="6"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="3"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="6"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="6"/>
+      <c r="B43" s="9"/>
       <c r="C43" s="3"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="6"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="3"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -984,7 +996,7 @@
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -992,13 +1004,13 @@
       </c>
     </row>
     <row r="47" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C47" s="3"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -1006,7 +1018,7 @@
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -1014,7 +1026,7 @@
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="6" t="s">
         <v>64</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -1022,34 +1034,53 @@
       </c>
     </row>
     <row r="51" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C51" s="3"/>
     </row>
     <row r="52" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C52" s="3"/>
     </row>
     <row r="53" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="3"/>
     </row>
     <row r="54" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C54" s="3"/>
     </row>
     <row r="55" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B56" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C58" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>